<commit_message>
updated files from canada
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pembinainstitute.sharepoint.com/sites/PRO-EnergyPolicySimulator2021/Shared Documents/Research and Analysis/CANADA-inputData/elec/BCpUC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{26C6F2EA-4A60-4C7E-ADE8-36917C57C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F58ACF7-5EDE-4072-8345-116694F51E0E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{26C6F2EA-4A60-4C7E-ADE8-36917C57C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40EB09E9-16D6-4F10-A52F-2BC22B003235}"/>
   <bookViews>
-    <workbookView xWindow="-13890" yWindow="-16365" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="BCpUC" sheetId="3" r:id="rId5"/>
     <sheet name="BBoSCpUC" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterate="1" iterateCount="25"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2334,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4 B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2567,6 +2567,7 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B29" r:id="rId3" xr:uid="{CA93FE29-A0A0-406A-B94C-DC5006AB819F}"/>
+    <hyperlink ref="B22" r:id="rId4" xr:uid="{D8978125-F17F-4A10-A9E4-25822C7EBF87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2577,7 +2578,7 @@
   <dimension ref="B1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5933,7 +5934,7 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6191,15 +6192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
@@ -6459,15 +6451,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04BE3C00-9504-4975-9E78-5F6466C59A6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A46C12-9FE6-4E9A-A53E-BF2A84A43F88}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6485,4 +6478,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04BE3C00-9504-4975-9E78-5F6466C59A6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated data from pembina
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26301"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -6193,15 +6193,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
@@ -6461,10 +6452,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04BE3C00-9504-4975-9E78-5F6466C59A6A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A46C12-9FE6-4E9A-A53E-BF2A84A43F88}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A46C12-9FE6-4E9A-A53E-BF2A84A43F88}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04BE3C00-9504-4975-9E78-5F6466C59A6A}"/>
 </file>
</xml_diff>